<commit_message>
bootstrap, figure formatting, table formatting
</commit_message>
<xml_diff>
--- a/tables/Table1/Table1.xlsx
+++ b/tables/Table1/Table1.xlsx
@@ -492,7 +492,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -510,7 +510,7 @@
         <v>0.97</v>
       </c>
       <c r="C2">
-        <v>2.0999999999999999E-3</v>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -521,7 +521,7 @@
         <v>0.91</v>
       </c>
       <c r="C3">
-        <v>3.5000000000000001E-3</v>
+        <v>8.6999999999999994E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -529,10 +529,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.57999999999999996</v>
+        <v>0.6</v>
       </c>
       <c r="C4">
-        <v>1.7000000000000001E-2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -540,11 +540,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <f>-0.62+E8</f>
-        <v>-0.62</v>
+        <v>-0.6</v>
       </c>
       <c r="C5">
-        <v>4.3999999999999997E-2</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>